<commit_message>
diagrama de atividade avaliar receita
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Confecionar Receita.xlsx
+++ b/Parte2/use_cases/Confecionar Receita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/Dolce_Cheferini/Parte2/use_cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/LI4/Parte2/use_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B2615-C53D-C54F-A57C-E22B808CA0CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC27A99-E1DC-2844-BDE2-F53F339096ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>2.3 Regressa a 1</t>
   </si>
   <si>
-    <t>3. Inicia temporizador para o passo</t>
-  </si>
-  <si>
     <t>4. Confirma realização do passo</t>
   </si>
   <si>
@@ -100,24 +97,12 @@
     <t>(1/2/3/4).2 Confirma ação sugerida</t>
   </si>
   <si>
-    <t>5. Apresenta informação comparativa entre a confeção do utilizador e o tempo de confeção esperado</t>
-  </si>
-  <si>
-    <t>6. &lt;&lt;include&gt;&gt; Avalia receita</t>
-  </si>
-  <si>
-    <t>7. Termina confeção</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Alternativa 1 [ação do passo suscita dúvidas] (Passo 1 e 2)</t>
   </si>
   <si>
     <t xml:space="preserve"> Alternativa 2 [aspecto final não corresponde à imagem apresentada] (Passo 2)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alternativa 3 [existem mais passos] (Passo 3)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Alternativa 4 [passo requer contagem de tempo] (Passo 4)</t>
   </si>
   <si>
@@ -128,6 +113,21 @@
   </si>
   <si>
     <t>3.1 Regista valor do temporizador</t>
+  </si>
+  <si>
+    <t>5. &lt;&lt;include&gt;&gt; Avalia receita</t>
+  </si>
+  <si>
+    <t>6. Termina confeção</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 3 [existem mais passos] (Passo 4)</t>
+  </si>
+  <si>
+    <t>3. Inicia cronómetro para o passo</t>
+  </si>
+  <si>
+    <t>4. Termina cronómetro para o passo</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -318,15 +318,6 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -389,12 +380,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,18 +402,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,40 +804,40 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -859,59 +848,58 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="17"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
+    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="13"/>
+      <c r="D11" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D13" s="8"/>
     </row>
     <row r="14" spans="2:5" ht="34.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
-        <v>27</v>
+      <c r="B14" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>13</v>
@@ -919,27 +907,27 @@
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="6"/>
       <c r="D15" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
-        <v>28</v>
+      <c r="B18" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>16</v>
@@ -947,97 +935,97 @@
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
-        <v>29</v>
+      <c r="B22" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="6"/>
       <c r="D23" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
-        <v>30</v>
+      <c r="B25" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="6"/>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="2:4" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="2:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
-        <v>31</v>
+      <c r="B28" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="B29" s="16"/>
+      <c r="C29" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="2:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="20"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B13"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Correção ao use case confecionar receita
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Confecionar Receita.xlsx
+++ b/Parte2/use_cases/Confecionar Receita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/LI4/Parte2/use_cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LI4\Parte2\use_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F3DF97-DB79-9E45-BE17-201ED133895C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2495533-A139-4F3C-949A-BEEF7CF8EAD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2900" windowWidth="21600" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>(1/2).1 Seleciona ação que suscita dúvidas</t>
   </si>
   <si>
-    <t>(1/2).2 &lt;&lt;include&gt;&gt; Apresenta informação extra relativa à ação selecionada</t>
-  </si>
-  <si>
     <t>(1/2).3 Regressa ao passo que estava a confecionar</t>
   </si>
   <si>
@@ -85,30 +82,18 @@
     <t>(1/2/3/4).2 Confirma ação sugerida</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alternativa 1 [ação do passo suscita dúvidas] (Passo 1 e 2)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Alternativa 4 [passo requer contagem de tempo] (Passo 4)</t>
   </si>
   <si>
     <t xml:space="preserve"> Alternativa 5 [temporizador decrescente chega a 0] (Passos 1,2,3,4)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alternativa 3 [existem mais passos] (Passo 4)</t>
-  </si>
-  <si>
     <t>3. Inicia temporizador para o passo</t>
   </si>
   <si>
     <t>(1/2/3/4).1 Alerta para fim da contagem e apresenta sugestão de ação</t>
   </si>
   <si>
-    <t>4.1 Regressa a 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alternativa 2 [aspecto final não corresponde à imagem apresentada] (Passo 4)</t>
-  </si>
-  <si>
     <t>4.1 Reinicia confeção de receita</t>
   </si>
   <si>
@@ -124,10 +109,25 @@
     <t>4.2 Atualiza número de tentativas de confeção</t>
   </si>
   <si>
-    <t>4.3 Regressa a 1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 1 [passo suscita dúvidas] (Passo 1 e 2)</t>
+  </si>
+  <si>
+    <t>(1/2).2 &lt;&lt;include&gt;&gt; Apresenta informação extra relativa ao passo selecionado</t>
+  </si>
+  <si>
+    <t>4.3 Regressa a Preparar Receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exceção 2 [aspecto final não corresponde à imagem apresentada] (Passo 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 3 [existem mais passos] (Passo 5)</t>
+  </si>
+  <si>
+    <t>5.1 Regressa a 1</t>
   </si>
 </sst>
 </file>
@@ -387,6 +387,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -398,12 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,57 +789,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="88" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
     <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.1640625" customWidth="1"/>
+    <col min="4" max="4" width="72.125" customWidth="1"/>
     <col min="5" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -849,185 +849,185 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
+    <row r="7" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="17"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
+    <row r="8" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="17"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
+    <row r="9" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="17"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="17"/>
       <c r="C10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
+    <row r="11" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="17"/>
       <c r="C11" s="6"/>
       <c r="D11" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="17"/>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
+    <row r="13" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="17"/>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:5" ht="34.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>19</v>
+    <row r="14" spans="2:5" ht="34.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="2:5" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
+    <row r="15" spans="2:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="17"/>
       <c r="C15" s="6"/>
       <c r="D15" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="17"/>
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="17"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
-        <v>26</v>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
+    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="17"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="17"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="17"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="17"/>
       <c r="C23" s="6"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15"/>
+    <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="17"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>20</v>
+    <row r="25" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="17"/>
       <c r="C26" s="6"/>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="2:4" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
+    <row r="27" spans="2:4" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="17"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="2:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
-        <v>21</v>
+    <row r="28" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="19"/>
       <c r="C29" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="2:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
+    <row r="30" spans="2:4" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="20"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>